<commit_message>
chore: updated meta key
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/out_meta_5_20.xlsx
+++ b/utils/localization/resources/backup/out_meta_5_20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/all_keys_generator/out/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D503FFD-DFE1-804B-A729-ECC1E09F33BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF63286F-11DC-4C4D-AE45-A2D9DB2A7E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6422" uniqueCount="3770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6422" uniqueCount="3771">
   <si>
     <t>Key</t>
   </si>
@@ -11330,6 +11330,9 @@
   </si>
   <si>
     <t>10 ವರ್ಷಗಳವರೆಗೆ</t>
+  </si>
+  <si>
+    <t>Your Language</t>
   </si>
 </sst>
 </file>
@@ -11694,11 +11697,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q470"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
-      <selection activeCell="K383" sqref="K383"/>
+    <sheetView tabSelected="1" topLeftCell="A630" workbookViewId="0">
+      <selection activeCell="A288" sqref="A288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -23968,7 +23974,7 @@
     </row>
     <row r="288" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>2397</v>
+        <v>3770</v>
       </c>
       <c r="B288" t="s">
         <v>2397</v>

</xml_diff>

<commit_message>
chore: added latest translation as of now
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/out_meta_5_20.xlsx
+++ b/utils/localization/resources/backup/out_meta_5_20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA7BA78-A2B0-9B44-A3B1-DA8EEC75AE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54BC716-9A91-6042-9AA9-24F64E350024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6446" uniqueCount="3799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6578" uniqueCount="3801">
   <si>
     <t>Key</t>
   </si>
@@ -11458,6 +11458,52 @@
   </si>
   <si>
     <t>An unexpected error has occurred.</t>
+  </si>
+  <si>
+    <r>
+      <t>Translated &lt;contribution-count&gt; &lt;language&gt; &lt;span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4A86E8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sentence(s)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Validated &lt;validation-count&gt; &lt;language&gt; &lt;span&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4A86E8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sentence(s)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;/span&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -11842,16 +11888,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q482"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A459" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A478" sqref="A478"/>
+      <selection pane="bottomLeft" activeCell="Q471" sqref="Q471:Q482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="60.83203125" style="2" customWidth="1"/>
-    <col min="3" max="17" width="46.6640625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="46.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="17" width="46.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
@@ -32065,6 +32112,39 @@
       <c r="B471" s="3" t="s">
         <v>3765</v>
       </c>
+      <c r="G471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="H471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="I471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="J471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="K471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="L471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="M471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="N471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="O471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="P471" s="3" t="s">
+        <v>3765</v>
+      </c>
+      <c r="Q471" s="3" t="s">
+        <v>3765</v>
+      </c>
     </row>
     <row r="472" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A472" s="2" t="s">
@@ -32073,6 +32153,39 @@
       <c r="B472" s="2" t="s">
         <v>3766</v>
       </c>
+      <c r="G472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="H472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="I472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="J472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="K472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="L472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="M472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="N472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="O472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="P472" s="2" t="s">
+        <v>3766</v>
+      </c>
+      <c r="Q472" s="2" t="s">
+        <v>3766</v>
+      </c>
     </row>
     <row r="473" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A473" s="2" t="s">
@@ -32081,6 +32194,39 @@
       <c r="B473" s="2" t="s">
         <v>3767</v>
       </c>
+      <c r="G473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="H473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="I473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="J473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="K473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="L473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="M473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="N473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="O473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="P473" s="2" t="s">
+        <v>3767</v>
+      </c>
+      <c r="Q473" s="2" t="s">
+        <v>3767</v>
+      </c>
     </row>
     <row r="474" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A474" s="2" t="s">
@@ -32089,6 +32235,39 @@
       <c r="B474" s="2" t="s">
         <v>3768</v>
       </c>
+      <c r="G474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="H474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="I474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="J474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="K474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="L474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="M474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="N474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="O474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="P474" s="2" t="s">
+        <v>3768</v>
+      </c>
+      <c r="Q474" s="2" t="s">
+        <v>3768</v>
+      </c>
     </row>
     <row r="475" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A475" s="3" t="s">
@@ -32097,6 +32276,39 @@
       <c r="B475" s="3" t="s">
         <v>3769</v>
       </c>
+      <c r="G475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="H475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="I475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="J475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="K475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="L475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="M475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="N475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="O475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="P475" s="3" t="s">
+        <v>3769</v>
+      </c>
+      <c r="Q475" s="3" t="s">
+        <v>3769</v>
+      </c>
     </row>
     <row r="476" spans="1:17" ht="17" x14ac:dyDescent="0.2">
       <c r="A476" s="3" t="s">
@@ -32105,20 +32317,119 @@
       <c r="B476" s="3" t="s">
         <v>3770</v>
       </c>
+      <c r="G476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="H476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="I476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="J476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="K476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="L476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="M476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="N476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="O476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="P476" s="3" t="s">
+        <v>3770</v>
+      </c>
+      <c r="Q476" s="3" t="s">
+        <v>3770</v>
+      </c>
     </row>
     <row r="477" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A477" s="3" t="s">
-        <v>3771</v>
+        <v>3799</v>
       </c>
       <c r="B477" s="3" t="s">
         <v>3771</v>
       </c>
+      <c r="G477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="H477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="I477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="J477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="K477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="L477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="M477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="N477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="O477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="P477" s="3" t="s">
+        <v>3771</v>
+      </c>
+      <c r="Q477" s="3" t="s">
+        <v>3771</v>
+      </c>
     </row>
     <row r="478" spans="1:17" ht="34" x14ac:dyDescent="0.2">
       <c r="A478" s="3" t="s">
+        <v>3800</v>
+      </c>
+      <c r="B478" s="3" t="s">
         <v>3772</v>
       </c>
-      <c r="B478" s="3" t="s">
+      <c r="G478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="H478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="I478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="J478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="K478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="L478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="M478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="N478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="O478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="P478" s="3" t="s">
+        <v>3772</v>
+      </c>
+      <c r="Q478" s="3" t="s">
         <v>3772</v>
       </c>
     </row>
@@ -32129,6 +32440,39 @@
       <c r="B479" s="3" t="s">
         <v>3796</v>
       </c>
+      <c r="G479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="H479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="I479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="J479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="K479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="L479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="M479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="N479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="O479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="P479" s="3" t="s">
+        <v>3796</v>
+      </c>
+      <c r="Q479" s="3" t="s">
+        <v>3796</v>
+      </c>
     </row>
     <row r="480" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A480" s="4" t="s">
@@ -32137,20 +32481,119 @@
       <c r="B480" s="4" t="s">
         <v>3797</v>
       </c>
-    </row>
-    <row r="481" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="G480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="H480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="I480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="J480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="K480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="L480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="M480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="N480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="O480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="P480" s="4" t="s">
+        <v>3797</v>
+      </c>
+      <c r="Q480" s="4" t="s">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="481" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A481" s="4" t="s">
         <v>3798</v>
       </c>
       <c r="B481" s="4" t="s">
         <v>3798</v>
       </c>
-    </row>
-    <row r="482" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="G481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="H481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="I481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="J481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="K481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="L481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="M481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="N481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="O481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="P481" s="4" t="s">
+        <v>3798</v>
+      </c>
+      <c r="Q481" s="4" t="s">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="482" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A482" s="4" t="s">
         <v>2871</v>
       </c>
       <c r="B482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="G482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="H482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="I482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="J482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="K482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="L482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="M482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="N482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="O482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="P482" s="4" t="s">
+        <v>2871</v>
+      </c>
+      <c r="Q482" s="4" t="s">
         <v>2871</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: added required keys and their translations for graphs and charts
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/out_meta_5_20.xlsx
+++ b/utils/localization/resources/backup/out_meta_5_20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1FC181-5931-0741-9B1C-E16AAC70450B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C81E22-A236-BE43-9E56-FE622E340C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6578" uniqueCount="3802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6604" uniqueCount="3804">
   <si>
     <t>Key</t>
   </si>
@@ -11500,6 +11500,12 @@
   </si>
   <si>
     <t>Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Month</t>
   </si>
 </sst>
 </file>
@@ -11882,19 +11888,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q482"/>
+  <dimension ref="A2:Q484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A339" sqref="A339"/>
+      <pane ySplit="2" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C483" sqref="C483:C484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="60.83203125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="46.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="17" width="46.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="62.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="2" customWidth="1"/>
+    <col min="6" max="17" width="46.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
@@ -32593,6 +32601,88 @@
         <v>2870</v>
       </c>
     </row>
+    <row r="483" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="B483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="G483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="H483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="I483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="J483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="K483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="L483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="M483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="N483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="O483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="P483" s="2" t="s">
+        <v>3802</v>
+      </c>
+      <c r="Q483" s="2" t="s">
+        <v>3802</v>
+      </c>
+    </row>
+    <row r="484" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="B484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="G484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="H484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="I484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="J484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="K484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="L484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="M484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="N484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="O484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="P484" s="2" t="s">
+        <v>3803</v>
+      </c>
+      <c r="Q484" s="2" t="s">
+        <v>3803</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: added translation and fixed thank you page message
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/out_meta_5_20.xlsx
+++ b/utils/localization/resources/backup/out_meta_5_20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C81E22-A236-BE43-9E56-FE622E340C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582D7954-1AC1-894C-8AE7-113623EF97F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6604" uniqueCount="3804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6630" uniqueCount="3806">
   <si>
     <t>Key</t>
   </si>
@@ -11506,6 +11506,12 @@
   </si>
   <si>
     <t>Month</t>
+  </si>
+  <si>
+    <t>We are processing multiple requests at the moment. Please try again after sometime.</t>
+  </si>
+  <si>
+    <t>No badge earned for &lt;initiative&gt;</t>
   </si>
 </sst>
 </file>
@@ -11888,24 +11894,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q484"/>
+  <dimension ref="A2:Q486"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C483" sqref="C483:C484"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G485" sqref="G485:Q486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="71" style="2" customWidth="1"/>
     <col min="2" max="2" width="62.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="2" customWidth="1"/>
-    <col min="6" max="17" width="46.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="46.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="17" width="46.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -12615,7 +12622,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>187</v>
       </c>
@@ -12659,7 +12666,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>200</v>
       </c>
@@ -12703,7 +12710,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>212</v>
       </c>
@@ -12747,7 +12754,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>224</v>
       </c>
@@ -12791,7 +12798,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>236</v>
       </c>
@@ -12835,7 +12842,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>248</v>
       </c>
@@ -12879,7 +12886,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>260</v>
       </c>
@@ -12923,7 +12930,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>272</v>
       </c>
@@ -12967,7 +12974,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>284</v>
       </c>
@@ -13011,7 +13018,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>296</v>
       </c>
@@ -13055,7 +13062,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>308</v>
       </c>
@@ -13099,7 +13106,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>320</v>
       </c>
@@ -13143,7 +13150,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>332</v>
       </c>
@@ -13187,7 +13194,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>344</v>
       </c>
@@ -13275,7 +13282,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>368</v>
       </c>
@@ -13319,7 +13326,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>375</v>
       </c>
@@ -13407,7 +13414,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>399</v>
       </c>
@@ -13451,7 +13458,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>410</v>
       </c>
@@ -13495,7 +13502,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>422</v>
       </c>
@@ -13539,7 +13546,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>434</v>
       </c>
@@ -13583,7 +13590,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>446</v>
       </c>
@@ -13627,7 +13634,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>459</v>
       </c>
@@ -13671,7 +13678,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>471</v>
       </c>
@@ -13715,7 +13722,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>483</v>
       </c>
@@ -13759,7 +13766,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>495</v>
       </c>
@@ -13806,7 +13813,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>509</v>
       </c>
@@ -13850,7 +13857,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>521</v>
       </c>
@@ -13894,7 +13901,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>532</v>
       </c>
@@ -13938,7 +13945,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>542</v>
       </c>
@@ -13982,7 +13989,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>552</v>
       </c>
@@ -14026,7 +14033,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>553</v>
       </c>
@@ -14070,7 +14077,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>563</v>
       </c>
@@ -14114,7 +14121,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>564</v>
       </c>
@@ -14158,7 +14165,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>576</v>
       </c>
@@ -14202,7 +14209,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>587</v>
       </c>
@@ -14331,7 +14338,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>603</v>
       </c>
@@ -14375,7 +14382,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>616</v>
       </c>
@@ -14674,7 +14681,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>659</v>
       </c>
@@ -14718,7 +14725,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>671</v>
       </c>
@@ -14762,7 +14769,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>683</v>
       </c>
@@ -14806,7 +14813,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>695</v>
       </c>
@@ -14935,7 +14942,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>709</v>
       </c>
@@ -15064,7 +15071,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>726</v>
       </c>
@@ -15108,7 +15115,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>739</v>
       </c>
@@ -15237,7 +15244,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>753</v>
       </c>
@@ -15281,7 +15288,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>754</v>
       </c>
@@ -15498,7 +15505,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="84" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>793</v>
       </c>
@@ -15542,7 +15549,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>794</v>
       </c>
@@ -15586,7 +15593,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="86" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>795</v>
       </c>
@@ -15671,7 +15678,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>797</v>
       </c>
@@ -15756,7 +15763,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>810</v>
       </c>
@@ -15800,7 +15807,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>811</v>
       </c>
@@ -15844,7 +15851,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>823</v>
       </c>
@@ -15929,7 +15936,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>837</v>
       </c>
@@ -15973,7 +15980,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>849</v>
       </c>
@@ -16061,7 +16068,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>873</v>
       </c>
@@ -16149,7 +16156,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>898</v>
       </c>
@@ -16237,7 +16244,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>922</v>
       </c>
@@ -16325,7 +16332,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>946</v>
       </c>
@@ -16413,7 +16420,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>972</v>
       </c>
@@ -16501,7 +16508,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>997</v>
       </c>
@@ -16791,7 +16798,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>1081</v>
       </c>
@@ -16835,7 +16842,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="115" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>1094</v>
       </c>
@@ -16879,7 +16886,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="116" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>1106</v>
       </c>
@@ -17509,7 +17516,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="131" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>1289</v>
       </c>
@@ -17553,7 +17560,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="132" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>1301</v>
       </c>
@@ -17597,7 +17604,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="133" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>1313</v>
       </c>
@@ -17641,7 +17648,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="134" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>1325</v>
       </c>
@@ -17685,7 +17692,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="135" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>1337</v>
       </c>
@@ -17811,7 +17818,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="138" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>1374</v>
       </c>
@@ -17855,7 +17862,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="139" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>1385</v>
       </c>
@@ -17940,7 +17947,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="141" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>1409</v>
       </c>
@@ -18028,7 +18035,7 @@
         <v>1433</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>1434</v>
       </c>
@@ -18072,7 +18079,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="144" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>1446</v>
       </c>
@@ -18116,7 +18123,7 @@
         <v>1457</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>1458</v>
       </c>
@@ -18406,7 +18413,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>1541</v>
       </c>
@@ -18494,7 +18501,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="154" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>1565</v>
       </c>
@@ -18538,7 +18545,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>1577</v>
       </c>
@@ -18582,7 +18589,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>1589</v>
       </c>
@@ -18626,7 +18633,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>1602</v>
       </c>
@@ -18670,7 +18677,7 @@
         <v>1613</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>1614</v>
       </c>
@@ -18714,7 +18721,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>1626</v>
       </c>
@@ -18758,7 +18765,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>1638</v>
       </c>
@@ -18802,7 +18809,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>1650</v>
       </c>
@@ -18846,7 +18853,7 @@
         <v>1661</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>1662</v>
       </c>
@@ -18890,7 +18897,7 @@
         <v>1673</v>
       </c>
     </row>
-    <row r="163" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>1674</v>
       </c>
@@ -18934,7 +18941,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>1686</v>
       </c>
@@ -18978,7 +18985,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>1698</v>
       </c>
@@ -19066,7 +19073,7 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>1721</v>
       </c>
@@ -19154,7 +19161,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>1745</v>
       </c>
@@ -19198,7 +19205,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>1757</v>
       </c>
@@ -19242,7 +19249,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>1769</v>
       </c>
@@ -19330,7 +19337,7 @@
         <v>1791</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>1792</v>
       </c>
@@ -19497,7 +19504,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="177" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>1807</v>
       </c>
@@ -19787,7 +19794,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>1825</v>
       </c>
@@ -20039,7 +20046,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>1853</v>
       </c>
@@ -20288,7 +20295,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="196" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
         <v>1870</v>
       </c>
@@ -20420,7 +20427,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="199" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>1897</v>
       </c>
@@ -21284,7 +21291,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="220" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A220" s="2" t="s">
         <v>1931</v>
       </c>
@@ -21492,7 +21499,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="225" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
         <v>1947</v>
       </c>
@@ -21782,7 +21789,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="232" spans="1:17" ht="80" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
         <v>1965</v>
       </c>
@@ -22028,7 +22035,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="238" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
         <v>1972</v>
       </c>
@@ -22072,7 +22079,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="239" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
         <v>1984</v>
       </c>
@@ -22116,7 +22123,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="240" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
         <v>1996</v>
       </c>
@@ -22160,7 +22167,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="241" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
         <v>2008</v>
       </c>
@@ -22245,7 +22252,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="243" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
         <v>2022</v>
       </c>
@@ -22289,7 +22296,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="244" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
         <v>2034</v>
       </c>
@@ -22333,7 +22340,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="245" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
         <v>2047</v>
       </c>
@@ -22377,7 +22384,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="246" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
         <v>2059</v>
       </c>
@@ -22503,7 +22510,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="249" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
         <v>2073</v>
       </c>
@@ -22547,7 +22554,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="250" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
         <v>2086</v>
       </c>
@@ -22632,7 +22639,7 @@
         <v>2099</v>
       </c>
     </row>
-    <row r="252" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
         <v>2100</v>
       </c>
@@ -22717,7 +22724,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="254" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
         <v>2114</v>
       </c>
@@ -22761,7 +22768,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="255" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
         <v>2125</v>
       </c>
@@ -22805,7 +22812,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="256" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
         <v>2136</v>
       </c>
@@ -22849,7 +22856,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="257" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
         <v>2146</v>
       </c>
@@ -22893,7 +22900,7 @@
         <v>2156</v>
       </c>
     </row>
-    <row r="258" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
         <v>2157</v>
       </c>
@@ -22937,7 +22944,7 @@
         <v>2167</v>
       </c>
     </row>
-    <row r="259" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
         <v>2168</v>
       </c>
@@ -22981,7 +22988,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="260" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
         <v>2178</v>
       </c>
@@ -23107,7 +23114,7 @@
         <v>2191</v>
       </c>
     </row>
-    <row r="263" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
         <v>2192</v>
       </c>
@@ -23397,7 +23404,7 @@
         <v>2242</v>
       </c>
     </row>
-    <row r="270" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
         <v>2243</v>
       </c>
@@ -23441,7 +23448,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="271" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
         <v>2255</v>
       </c>
@@ -23485,7 +23492,7 @@
         <v>2266</v>
       </c>
     </row>
-    <row r="272" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A272" s="2" t="s">
         <v>2267</v>
       </c>
@@ -23529,7 +23536,7 @@
         <v>2279</v>
       </c>
     </row>
-    <row r="273" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A273" s="2" t="s">
         <v>2280</v>
       </c>
@@ -23614,7 +23621,7 @@
         <v>2292</v>
       </c>
     </row>
-    <row r="275" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A275" s="2" t="s">
         <v>2293</v>
       </c>
@@ -23658,7 +23665,7 @@
         <v>2301</v>
       </c>
     </row>
-    <row r="276" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A276" s="2" t="s">
         <v>2302</v>
       </c>
@@ -23702,7 +23709,7 @@
         <v>2314</v>
       </c>
     </row>
-    <row r="277" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A277" s="2" t="s">
         <v>2315</v>
       </c>
@@ -23787,7 +23794,7 @@
         <v>2327</v>
       </c>
     </row>
-    <row r="279" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A279" s="2" t="s">
         <v>2328</v>
       </c>
@@ -23831,7 +23838,7 @@
         <v>2339</v>
       </c>
     </row>
-    <row r="280" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A280" s="2" t="s">
         <v>2340</v>
       </c>
@@ -23875,7 +23882,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="281" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A281" s="2" t="s">
         <v>2351</v>
       </c>
@@ -24042,7 +24049,7 @@
         <v>2365</v>
       </c>
     </row>
-    <row r="285" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
         <v>2366</v>
       </c>
@@ -24086,7 +24093,7 @@
         <v>2377</v>
       </c>
     </row>
-    <row r="286" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A286" s="2" t="s">
         <v>2378</v>
       </c>
@@ -24622,7 +24629,7 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="299" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A299" s="2" t="s">
         <v>2402</v>
       </c>
@@ -25293,7 +25300,7 @@
         <v>2472</v>
       </c>
     </row>
-    <row r="315" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A315" s="2" t="s">
         <v>2473</v>
       </c>
@@ -25337,7 +25344,7 @@
         <v>2484</v>
       </c>
     </row>
-    <row r="316" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A316" s="2" t="s">
         <v>2485</v>
       </c>
@@ -25381,7 +25388,7 @@
         <v>2494</v>
       </c>
     </row>
-    <row r="317" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A317" s="2" t="s">
         <v>2495</v>
       </c>
@@ -25425,7 +25432,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="318" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A318" s="2" t="s">
         <v>2507</v>
       </c>
@@ -25469,7 +25476,7 @@
         <v>2518</v>
       </c>
     </row>
-    <row r="319" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A319" s="2" t="s">
         <v>2519</v>
       </c>
@@ -25513,7 +25520,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="320" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A320" s="2" t="s">
         <v>2530</v>
       </c>
@@ -25689,7 +25696,7 @@
         <v>2570</v>
       </c>
     </row>
-    <row r="324" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A324" s="2" t="s">
         <v>6</v>
       </c>
@@ -26041,7 +26048,7 @@
         <v>2653</v>
       </c>
     </row>
-    <row r="332" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A332" s="2" t="s">
         <v>2654</v>
       </c>
@@ -26085,7 +26092,7 @@
         <v>2664</v>
       </c>
     </row>
-    <row r="333" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A333" s="2" t="s">
         <v>2665</v>
       </c>
@@ -26129,7 +26136,7 @@
         <v>2675</v>
       </c>
     </row>
-    <row r="334" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A334" s="2" t="s">
         <v>2676</v>
       </c>
@@ -26173,7 +26180,7 @@
         <v>2687</v>
       </c>
     </row>
-    <row r="335" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A335" s="2" t="s">
         <v>2688</v>
       </c>
@@ -27737,7 +27744,7 @@
         <v>2746</v>
       </c>
     </row>
-    <row r="373" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A373" s="2" t="s">
         <v>2747</v>
       </c>
@@ -27828,7 +27835,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="375" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A375" s="2" t="s">
         <v>2773</v>
       </c>
@@ -28083,7 +28090,7 @@
         <v>2845</v>
       </c>
     </row>
-    <row r="381" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A381" s="2" t="s">
         <v>2846</v>
       </c>
@@ -28130,7 +28137,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="382" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A382" s="2" t="s">
         <v>2848</v>
       </c>
@@ -28174,7 +28181,7 @@
         <v>2859</v>
       </c>
     </row>
-    <row r="383" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A383" s="2" t="s">
         <v>2860</v>
       </c>
@@ -28218,7 +28225,7 @@
         <v>2869</v>
       </c>
     </row>
-    <row r="384" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A384" s="2" t="s">
         <v>2870</v>
       </c>
@@ -28303,7 +28310,7 @@
         <v>2893</v>
       </c>
     </row>
-    <row r="386" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A386" s="2" t="s">
         <v>2894</v>
       </c>
@@ -28391,7 +28398,7 @@
         <v>2917</v>
       </c>
     </row>
-    <row r="388" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A388" s="2" t="s">
         <v>2918</v>
       </c>
@@ -28435,7 +28442,7 @@
         <v>2928</v>
       </c>
     </row>
-    <row r="389" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A389" s="2" t="s">
         <v>2929</v>
       </c>
@@ -28479,7 +28486,7 @@
         <v>2939</v>
       </c>
     </row>
-    <row r="390" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A390" s="2" t="s">
         <v>2940</v>
       </c>
@@ -28846,7 +28853,7 @@
         <v>3028</v>
       </c>
     </row>
-    <row r="398" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A398" s="2" t="s">
         <v>3029</v>
       </c>
@@ -28890,7 +28897,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="399" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A399" s="2" t="s">
         <v>3041</v>
       </c>
@@ -28934,7 +28941,7 @@
         <v>3052</v>
       </c>
     </row>
-    <row r="400" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A400" s="2" t="s">
         <v>3053</v>
       </c>
@@ -29019,7 +29026,7 @@
         <v>3075</v>
       </c>
     </row>
-    <row r="402" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A402" s="2" t="s">
         <v>3076</v>
       </c>
@@ -29189,7 +29196,7 @@
         <v>3121</v>
       </c>
     </row>
-    <row r="406" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A406" s="2" t="s">
         <v>3122</v>
       </c>
@@ -29233,7 +29240,7 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="407" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A407" s="2" t="s">
         <v>3133</v>
       </c>
@@ -29277,7 +29284,7 @@
         <v>3144</v>
       </c>
     </row>
-    <row r="408" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A408" s="2" t="s">
         <v>3145</v>
       </c>
@@ -29321,7 +29328,7 @@
         <v>3156</v>
       </c>
     </row>
-    <row r="409" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A409" s="2" t="s">
         <v>3157</v>
       </c>
@@ -29365,7 +29372,7 @@
         <v>3168</v>
       </c>
     </row>
-    <row r="410" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A410" s="2" t="s">
         <v>3169</v>
       </c>
@@ -29409,7 +29416,7 @@
         <v>3180</v>
       </c>
     </row>
-    <row r="411" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A411" s="2" t="s">
         <v>3181</v>
       </c>
@@ -29494,7 +29501,7 @@
         <v>3203</v>
       </c>
     </row>
-    <row r="413" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A413" s="2" t="s">
         <v>3204</v>
       </c>
@@ -29538,7 +29545,7 @@
         <v>3204</v>
       </c>
     </row>
-    <row r="414" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A414" s="2" t="s">
         <v>3206</v>
       </c>
@@ -29582,7 +29589,7 @@
         <v>3217</v>
       </c>
     </row>
-    <row r="415" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A415" s="2" t="s">
         <v>3218</v>
       </c>
@@ -29626,7 +29633,7 @@
         <v>3229</v>
       </c>
     </row>
-    <row r="416" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A416" s="2" t="s">
         <v>3230</v>
       </c>
@@ -29670,7 +29677,7 @@
         <v>3241</v>
       </c>
     </row>
-    <row r="417" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A417" s="2" t="s">
         <v>3242</v>
       </c>
@@ -29714,7 +29721,7 @@
         <v>3253</v>
       </c>
     </row>
-    <row r="418" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A418" s="2" t="s">
         <v>3254</v>
       </c>
@@ -29802,7 +29809,7 @@
         <v>3277</v>
       </c>
     </row>
-    <row r="420" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A420" s="2" t="s">
         <v>3278</v>
       </c>
@@ -29846,7 +29853,7 @@
         <v>3289</v>
       </c>
     </row>
-    <row r="421" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A421" s="2" t="s">
         <v>3290</v>
       </c>
@@ -29890,7 +29897,7 @@
         <v>3301</v>
       </c>
     </row>
-    <row r="422" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A422" s="2" t="s">
         <v>3302</v>
       </c>
@@ -29934,7 +29941,7 @@
         <v>3313</v>
       </c>
     </row>
-    <row r="423" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A423" s="2" t="s">
         <v>3314</v>
       </c>
@@ -29978,7 +29985,7 @@
         <v>3322</v>
       </c>
     </row>
-    <row r="424" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A424" s="2" t="s">
         <v>3323</v>
       </c>
@@ -30022,7 +30029,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row r="425" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A425" s="2" t="s">
         <v>3331</v>
       </c>
@@ -30066,7 +30073,7 @@
         <v>3340</v>
       </c>
     </row>
-    <row r="426" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A426" s="2" t="s">
         <v>3341</v>
       </c>
@@ -30110,7 +30117,7 @@
         <v>3351</v>
       </c>
     </row>
-    <row r="427" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A427" s="2" t="s">
         <v>3352</v>
       </c>
@@ -30289,7 +30296,7 @@
         <v>3389</v>
       </c>
     </row>
-    <row r="431" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A431" s="2" t="s">
         <v>3391</v>
       </c>
@@ -30333,7 +30340,7 @@
         <v>3402</v>
       </c>
     </row>
-    <row r="432" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A432" s="2" t="s">
         <v>3403</v>
       </c>
@@ -30427,7 +30434,7 @@
         <v>3429</v>
       </c>
     </row>
-    <row r="434" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A434" s="2" t="s">
         <v>3430</v>
       </c>
@@ -30477,7 +30484,7 @@
         <v>3442</v>
       </c>
     </row>
-    <row r="435" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A435" s="2" t="s">
         <v>3443</v>
       </c>
@@ -30521,7 +30528,7 @@
         <v>3454</v>
       </c>
     </row>
-    <row r="436" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A436" s="2" t="s">
         <v>3455</v>
       </c>
@@ -30665,7 +30672,7 @@
         <v>3494</v>
       </c>
     </row>
-    <row r="439" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A439" s="2" t="s">
         <v>3495</v>
       </c>
@@ -30947,7 +30954,7 @@
         <v>3570</v>
       </c>
     </row>
-    <row r="445" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A445" s="2" t="s">
         <v>3571</v>
       </c>
@@ -30991,7 +30998,7 @@
         <v>3582</v>
       </c>
     </row>
-    <row r="446" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A446" s="2" t="s">
         <v>3583</v>
       </c>
@@ -31117,7 +31124,7 @@
         <v>3615</v>
       </c>
     </row>
-    <row r="449" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A449" s="2" t="s">
         <v>3616</v>
       </c>
@@ -31161,7 +31168,7 @@
         <v>3628</v>
       </c>
     </row>
-    <row r="450" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A450" s="2" t="s">
         <v>3629</v>
       </c>
@@ -31246,7 +31253,7 @@
         <v>3650</v>
       </c>
     </row>
-    <row r="452" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A452" s="2" t="s">
         <v>3651</v>
       </c>
@@ -31290,7 +31297,7 @@
         <v>3662</v>
       </c>
     </row>
-    <row r="453" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A453" s="2" t="s">
         <v>3663</v>
       </c>
@@ -31434,7 +31441,7 @@
         <v>3702</v>
       </c>
     </row>
-    <row r="456" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A456" s="2" t="s">
         <v>3703</v>
       </c>
@@ -31584,7 +31591,7 @@
         <v>3739</v>
       </c>
     </row>
-    <row r="459" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A459" s="2" t="s">
         <v>3740</v>
       </c>
@@ -31628,7 +31635,7 @@
         <v>3740</v>
       </c>
     </row>
-    <row r="460" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A460" s="2" t="s">
         <v>3741</v>
       </c>
@@ -31672,7 +31679,7 @@
         <v>3741</v>
       </c>
     </row>
-    <row r="461" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A461" s="2" t="s">
         <v>3742</v>
       </c>
@@ -31716,7 +31723,7 @@
         <v>3742</v>
       </c>
     </row>
-    <row r="462" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A462" s="2" t="s">
         <v>3743</v>
       </c>
@@ -31848,7 +31855,7 @@
         <v>3745</v>
       </c>
     </row>
-    <row r="465" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A465" s="2" t="s">
         <v>3746</v>
       </c>
@@ -31892,7 +31899,7 @@
         <v>3746</v>
       </c>
     </row>
-    <row r="466" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A466" s="2" t="s">
         <v>3747</v>
       </c>
@@ -31936,7 +31943,7 @@
         <v>3747</v>
       </c>
     </row>
-    <row r="467" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A467" s="2" t="s">
         <v>3748</v>
       </c>
@@ -31980,7 +31987,7 @@
         <v>3748</v>
       </c>
     </row>
-    <row r="468" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A468" s="2" t="s">
         <v>3749</v>
       </c>
@@ -32024,7 +32031,7 @@
         <v>3749</v>
       </c>
     </row>
-    <row r="469" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A469" s="2" t="s">
         <v>3750</v>
       </c>
@@ -32681,6 +32688,88 @@
       </c>
       <c r="Q484" s="2" t="s">
         <v>3803</v>
+      </c>
+    </row>
+    <row r="485" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="B485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="G485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="H485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="I485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="J485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="K485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="L485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="M485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="N485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="O485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="P485" t="s">
+        <v>3804</v>
+      </c>
+      <c r="Q485" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="486" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="B486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="G486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="H486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="I486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="J486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="K486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="L486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="M486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="N486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="O486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="P486" t="s">
+        <v>3805</v>
+      </c>
+      <c r="Q486" t="s">
+        <v>3805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(translations): update translations 15 november
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/out_meta_5_20.xlsx
+++ b/utils/localization/resources/backup/out_meta_5_20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54C6BB1-0197-2642-B68C-9EB2FDBA554B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5216F35-3729-DF41-A948-3DD5A9D14359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6630" uniqueCount="3806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6773" uniqueCount="3821">
   <si>
     <t>Key</t>
   </si>
@@ -11513,12 +11513,57 @@
   <si>
     <t>I've contributed towards building open language repository for India on https://bhashini.gov.in/bhashadaan. &lt;x&gt; ranks &lt;y&gt; on &lt;initiative name&gt;. Let's make a difference by contributing to Bhasha Daan and empower our languages.</t>
   </si>
+  <si>
+    <t>Contribute to keep your language on top</t>
+  </si>
+  <si>
+    <t>Validate to keep your language on top</t>
+  </si>
+  <si>
+    <t>Please don't use only numerics or email as username</t>
+  </si>
+  <si>
+    <t>Only 1000 characters allowed</t>
+  </si>
+  <si>
+    <t>Contribute to see your language on top</t>
+  </si>
+  <si>
+    <t>Validate to see your language on top</t>
+  </si>
+  <si>
+    <t>We feel the text you entered doesn't match the original text, are you sure about your edit</t>
+  </si>
+  <si>
+    <t>404 Error</t>
+  </si>
+  <si>
+    <t>Seems this page doesn't exist</t>
+  </si>
+  <si>
+    <t>Visit our homepage</t>
+  </si>
+  <si>
+    <t>Unspecified location</t>
+  </si>
+  <si>
+    <t>Contribute to keep your language on top.</t>
+  </si>
+  <si>
+    <t>Validate to keep your language on top.</t>
+  </si>
+  <si>
+    <t>Contribute to see your language on top.</t>
+  </si>
+  <si>
+    <t>Validate to see your language on top.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11543,6 +11588,12 @@
       <color rgb="FF4A86E8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -11894,11 +11945,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q486"/>
+  <dimension ref="A2:Q497"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B232" sqref="B232"/>
+      <pane ySplit="2" topLeftCell="A478" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A501" sqref="A501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32772,7 +32823,459 @@
         <v>3803</v>
       </c>
     </row>
+    <row r="487" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A487" t="s">
+        <v>3817</v>
+      </c>
+      <c r="B487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="G487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="H487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="I487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="J487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="K487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="L487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="M487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="N487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="O487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="P487" t="s">
+        <v>3806</v>
+      </c>
+      <c r="Q487" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="488" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A488" t="s">
+        <v>3818</v>
+      </c>
+      <c r="B488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="G488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="H488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="I488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="J488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="K488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="L488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="M488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="N488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="O488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="P488" t="s">
+        <v>3807</v>
+      </c>
+      <c r="Q488" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="489" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="B489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="G489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="H489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="I489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="J489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="K489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="L489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="M489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="N489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="O489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="P489" t="s">
+        <v>3808</v>
+      </c>
+      <c r="Q489" t="s">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="490" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="B490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="G490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="H490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="I490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="J490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="K490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="L490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="M490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="N490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="O490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="P490" t="s">
+        <v>3809</v>
+      </c>
+      <c r="Q490" t="s">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="491" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A491" t="s">
+        <v>3819</v>
+      </c>
+      <c r="B491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="G491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="H491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="I491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="J491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="K491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="L491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="M491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="N491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="O491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="P491" t="s">
+        <v>3810</v>
+      </c>
+      <c r="Q491" t="s">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="492" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A492" t="s">
+        <v>3820</v>
+      </c>
+      <c r="B492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="G492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="H492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="I492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="J492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="K492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="L492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="M492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="N492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="O492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="P492" t="s">
+        <v>3811</v>
+      </c>
+      <c r="Q492" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="493" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="B493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="G493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="H493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="I493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="J493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="K493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="L493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="M493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="N493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="O493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="P493" t="s">
+        <v>3812</v>
+      </c>
+      <c r="Q493" t="s">
+        <v>3812</v>
+      </c>
+    </row>
+    <row r="494" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="B494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="G494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="H494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="I494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="J494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="K494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="L494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="M494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="N494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="O494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="P494" t="s">
+        <v>3813</v>
+      </c>
+      <c r="Q494" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="495" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="B495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="G495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="H495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="I495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="J495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="K495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="L495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="M495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="N495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="O495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="P495" t="s">
+        <v>3814</v>
+      </c>
+      <c r="Q495" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="496" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="B496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="G496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="H496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="I496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="J496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="K496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="L496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="M496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="N496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="O496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="P496" t="s">
+        <v>3815</v>
+      </c>
+      <c r="Q496" t="s">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="497" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="B497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="G497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="H497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="I497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="J497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="K497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="L497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="M497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="N497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="O497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="P497" t="s">
+        <v>3816</v>
+      </c>
+      <c r="Q497" t="s">
+        <v>3816</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore(translations): load latest translations november 18
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/out_meta_5_20.xlsx
+++ b/utils/localization/resources/backup/out_meta_5_20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-bhashadaan/utils/localization/resources/backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5216F35-3729-DF41-A948-3DD5A9D14359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF1294E-171A-834B-A221-EEF158877173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11532,9 +11532,6 @@
     <t>Validate to see your language on top</t>
   </si>
   <si>
-    <t>We feel the text you entered doesn't match the original text, are you sure about your edit</t>
-  </si>
-  <si>
     <t>404 Error</t>
   </si>
   <si>
@@ -11557,6 +11554,9 @@
   </si>
   <si>
     <t>Validate to see your language on top.</t>
+  </si>
+  <si>
+    <t>We feel the text you entered doesn't match the original text, are you sure about your edit?</t>
   </si>
 </sst>
 </file>
@@ -11948,18 +11948,18 @@
   <dimension ref="A2:Q497"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A478" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A501" sqref="A501"/>
+      <pane ySplit="2" topLeftCell="A467" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B484" sqref="B484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71" style="2" customWidth="1"/>
-    <col min="2" max="2" width="62.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="46.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="94.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.5" style="2" customWidth="1"/>
     <col min="7" max="17" width="46.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32825,7 +32825,7 @@
     </row>
     <row r="487" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
-        <v>3817</v>
+        <v>3816</v>
       </c>
       <c r="B487" t="s">
         <v>3806</v>
@@ -32866,7 +32866,7 @@
     </row>
     <row r="488" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
-        <v>3818</v>
+        <v>3817</v>
       </c>
       <c r="B488" t="s">
         <v>3807</v>
@@ -32989,7 +32989,7 @@
     </row>
     <row r="491" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
-        <v>3819</v>
+        <v>3818</v>
       </c>
       <c r="B491" t="s">
         <v>3810</v>
@@ -33030,7 +33030,7 @@
     </row>
     <row r="492" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
-        <v>3820</v>
+        <v>3819</v>
       </c>
       <c r="B492" t="s">
         <v>3811</v>
@@ -33071,207 +33071,211 @@
     </row>
     <row r="493" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="B493" t="s">
-        <v>3812</v>
-      </c>
+        <v>3820</v>
+      </c>
+      <c r="C493"/>
+      <c r="D493"/>
+      <c r="E493"/>
+      <c r="F493"/>
       <c r="G493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="H493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="I493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="J493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="K493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="L493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="M493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="N493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="O493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="P493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
       <c r="Q493" t="s">
-        <v>3812</v>
+        <v>3820</v>
       </c>
     </row>
     <row r="494" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="B494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="G494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="H494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="I494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="J494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="K494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="L494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="M494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="N494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="O494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="P494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
       <c r="Q494" t="s">
-        <v>3813</v>
+        <v>3812</v>
       </c>
     </row>
     <row r="495" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="B495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="G495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="H495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="I495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="J495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="K495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="L495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="M495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="N495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="O495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="P495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
       <c r="Q495" t="s">
-        <v>3814</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="496" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="B496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="G496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="H496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="I496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="J496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="K496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="L496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="M496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="N496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="O496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="P496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
       <c r="Q496" t="s">
-        <v>3815</v>
+        <v>3814</v>
       </c>
     </row>
     <row r="497" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="B497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="G497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="H497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="I497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="J497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="K497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="L497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="M497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="N497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="O497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="P497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
       <c r="Q497" t="s">
-        <v>3816</v>
+        <v>3815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>